<commit_message>
Group project US 9 and US10
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/HrmsTestData.xlsx
+++ b/src/test/resources/testdata/HrmsTestData.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gulen\eclipse-workspace\HrmsFramework\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gulen\eclipse-workspace\HrmsCucumberFrameworkMaven\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1808299E-6795-476C-B006-2BFDB450AD2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55A3902-441E-41C5-B0F8-B1955BB655A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12420" yWindow="0" windowWidth="16452" windowHeight="10152" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="AddEmployee" sheetId="2" r:id="rId2"/>
+    <sheet name="EmployeeLoginCredentials" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="3" r:id="rId2"/>
+    <sheet name="AddReport" sheetId="4" r:id="rId3"/>
+    <sheet name="AddEmployee" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>FirstName</t>
   </si>
@@ -40,55 +42,61 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Lastname</t>
-  </si>
-  <si>
-    <t>Middlename</t>
-  </si>
-  <si>
-    <t>Firstname</t>
-  </si>
-  <si>
-    <t>Johnn</t>
-  </si>
-  <si>
-    <t>Janee</t>
-  </si>
-  <si>
-    <t>Mx</t>
-  </si>
-  <si>
-    <t>Hx</t>
-  </si>
-  <si>
-    <t>Smithx</t>
-  </si>
-  <si>
-    <t>Mayax</t>
-  </si>
-  <si>
-    <t>Norax</t>
-  </si>
-  <si>
-    <t>Naomix</t>
-  </si>
-  <si>
-    <t>Felixx</t>
-  </si>
-  <si>
-    <t>Heightx</t>
-  </si>
-  <si>
-    <t>Faradayx</t>
-  </si>
-  <si>
-    <t>Adminx</t>
-  </si>
-  <si>
-    <t>Royal1235x</t>
-  </si>
-  <si>
     <t>admin123_@H</t>
+  </si>
+  <si>
+    <t>Adminxm</t>
+  </si>
+  <si>
+    <t>Royal1235xm</t>
+  </si>
+  <si>
+    <t>Mayaxm</t>
+  </si>
+  <si>
+    <t>Naomixm</t>
+  </si>
+  <si>
+    <t>Noraxm</t>
+  </si>
+  <si>
+    <t>Felixxm</t>
+  </si>
+  <si>
+    <t>Heightxm</t>
+  </si>
+  <si>
+    <t>Faradayxm</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t>Johnnn</t>
+  </si>
+  <si>
+    <t>Janeee</t>
+  </si>
+  <si>
+    <t>Mxx</t>
+  </si>
+  <si>
+    <t>Hxx</t>
+  </si>
+  <si>
+    <t>Smithxx</t>
+  </si>
+  <si>
+    <t>Report Name</t>
+  </si>
+  <si>
+    <t>Selection Criteria</t>
+  </si>
+  <si>
+    <t>Selected Criteria Include</t>
+  </si>
+  <si>
+    <t>Fields</t>
   </si>
 </sst>
 </file>
@@ -102,13 +110,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="16"/>
@@ -130,6 +131,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aharoni"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -150,14 +156,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -441,16 +447,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="17" style="2"/>
+    <col min="1" max="1" width="24.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="17" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,45 +476,45 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>20</v>
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>20</v>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -518,6 +529,54 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D8F7921-DED6-4379-9843-917CBBD18E81}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF0CF4F-1340-46C7-A119-5B09383EC7EC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2195B679-85ED-4EF8-879C-4525BB4B020A}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -527,40 +586,42 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.77734375" defaultRowHeight="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" width="16.77734375" style="3"/>
+    <col min="1" max="1" width="16.77734375" style="2"/>
+    <col min="2" max="2" width="21.109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="16.77734375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
+      <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
+      <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>